<commit_message>
Update CT Project Plan 6-26-2020.xlsx
</commit_message>
<xml_diff>
--- a/Week4 Pre/CT Project Plan 6-26-2020.xlsx
+++ b/Week4 Pre/CT Project Plan 6-26-2020.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A8515F-D382-BD42-9533-32A596973754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDCA6B7-66CE-4A15-8394-6D937D3A20DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16080" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-104" yWindow="-104" windowWidth="26728" windowHeight="14525" tabRatio="415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt" sheetId="11" r:id="rId1"/>
@@ -871,6 +871,15 @@
   </cellStyles>
   <dxfs count="79">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9948118533890809E-2"/>
@@ -1196,15 +1205,6 @@
           <color theme="0"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2513,15 +2513,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>25400</xdr:colOff>
+          <xdr:colOff>26314</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>63500</xdr:rowOff>
+          <xdr:rowOff>65784</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>63</xdr:col>
-          <xdr:colOff>228600</xdr:colOff>
+          <xdr:colOff>230245</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>241300</xdr:rowOff>
+          <xdr:rowOff>243401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2572,9 +2572,9 @@
     <filterColumn colId="5" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name="Category" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{EE48C34E-B98C-4BBA-90C8-388E8655DD6D}" name="Milestone Description" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{B8ACC97F-C189-49BA-91CF-CB5671185BCF}" name="Category" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{5419FA1B-A035-4F0A-9257-1AA4BCB5E6CF}" name="Assigned To" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{A60A6524-18F0-48B7-BB3C-2F4A35799FF7}" name="Progress"/>
     <tableColumn id="5" xr3:uid="{59612C1F-9AAB-483B-A6A5-3563E9D77941}" name="Start" dataCellStyle="Date"/>
     <tableColumn id="6" xr3:uid="{012C59F1-49D4-4A67-B8DD-855C6581FD6A}" name="No. Days" dataCellStyle="Comma [0]"/>
@@ -2856,25 +2856,25 @@
   </sheetPr>
   <dimension ref="A1:BL52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30.05" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" style="53" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.5" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" customWidth="1"/>
-    <col min="9" max="64" width="3.5" customWidth="1"/>
-    <col min="69" max="70" width="10.33203125"/>
+    <col min="1" max="1" width="2.6328125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" style="53" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.453125" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" customWidth="1"/>
+    <col min="8" max="8" width="2.6328125" customWidth="1"/>
+    <col min="9" max="64" width="3.453125" customWidth="1"/>
+    <col min="69" max="70" width="10.36328125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="15" t="s">
         <v>27</v>
       </c>
@@ -2913,7 +2913,7 @@
       <c r="AF1" s="20"/>
       <c r="AG1" s="20"/>
     </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="15" t="s">
         <v>19</v>
       </c>
@@ -2957,7 +2957,7 @@
       <c r="AE2" s="59"/>
       <c r="AF2" s="59"/>
     </row>
-    <row r="3" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>28</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="G3" s="64"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="15" t="s">
         <v>20</v>
       </c>
@@ -3067,7 +3067,7 @@
       <c r="BK4" s="41"/>
       <c r="BL4" s="41"/>
     </row>
-    <row r="5" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" ht="15.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>21</v>
       </c>
@@ -3303,7 +3303,7 @@
         <v>44038</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:64" s="20" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
@@ -3371,7 +3371,7 @@
       <c r="BK6" s="44"/>
       <c r="BL6" s="45"/>
     </row>
-    <row r="7" spans="1:64" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
         <v>23</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="8" spans="1:64" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" ht="30.05" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="BK8" s="35"/>
       <c r="BL8" s="35"/>
     </row>
-    <row r="9" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="15"/>
       <c r="B10" s="49" t="s">
         <v>42</v>
@@ -4170,7 +4170,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="15"/>
       <c r="B11" s="49" t="s">
         <v>43</v>
@@ -4416,7 +4416,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="15"/>
       <c r="B12" s="49" t="s">
         <v>56</v>
@@ -4494,7 +4494,7 @@
       <c r="BK12" s="37"/>
       <c r="BL12" s="37"/>
     </row>
-    <row r="13" spans="1:64" s="2" customFormat="1" ht="33.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" s="2" customFormat="1" ht="33.299999999999997" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="49" t="s">
         <v>44</v>
@@ -4740,7 +4740,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="49" t="s">
         <v>58</v>
@@ -4983,7 +4983,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14"/>
       <c r="B15" s="49" t="s">
         <v>62</v>
@@ -5061,7 +5061,7 @@
       <c r="BK15" s="37"/>
       <c r="BL15" s="37"/>
     </row>
-    <row r="16" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="14"/>
       <c r="B16" s="49" t="s">
         <v>59</v>
@@ -5139,7 +5139,7 @@
       <c r="BK16" s="37"/>
       <c r="BL16" s="37"/>
     </row>
-    <row r="17" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="49" t="s">
         <v>63</v>
@@ -5217,7 +5217,7 @@
       <c r="BK17" s="37"/>
       <c r="BL17" s="37"/>
     </row>
-    <row r="18" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="49" t="s">
         <v>61</v>
@@ -5295,7 +5295,7 @@
       <c r="BK18" s="37"/>
       <c r="BL18" s="37"/>
     </row>
-    <row r="19" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="49" t="s">
         <v>45</v>
@@ -5541,7 +5541,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="55" t="s">
         <v>64</v>
@@ -5609,7 +5609,7 @@
       <c r="BK20" s="37"/>
       <c r="BL20" s="37"/>
     </row>
-    <row r="21" spans="1:64" s="2" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:64" s="2" customFormat="1" ht="26.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="15"/>
       <c r="B21" s="49" t="s">
         <v>65</v>
@@ -5687,7 +5687,7 @@
       <c r="BK21" s="37"/>
       <c r="BL21" s="37"/>
     </row>
-    <row r="22" spans="1:64" s="2" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:64" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="15"/>
       <c r="B22" s="49" t="s">
         <v>66</v>
@@ -5768,7 +5768,7 @@
       <c r="BK22" s="37"/>
       <c r="BL22" s="37"/>
     </row>
-    <row r="23" spans="1:64" s="2" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:64" s="2" customFormat="1" ht="30.6" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="15"/>
       <c r="B23" s="49" t="s">
         <v>67</v>
@@ -5849,7 +5849,7 @@
       <c r="BK23" s="37"/>
       <c r="BL23" s="37"/>
     </row>
-    <row r="24" spans="1:64" s="2" customFormat="1" ht="34.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:64" s="2" customFormat="1" ht="34.700000000000003" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="15"/>
       <c r="B24" s="49" t="s">
         <v>68</v>
@@ -5927,7 +5927,7 @@
       <c r="BK24" s="37"/>
       <c r="BL24" s="37"/>
     </row>
-    <row r="25" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="55" t="s">
         <v>35</v>
@@ -6160,7 +6160,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:64" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:64" s="2" customFormat="1" ht="51.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="49" t="s">
         <v>46</v>
@@ -6403,7 +6403,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="B27" s="49" t="s">
         <v>47</v>
@@ -6415,7 +6415,7 @@
         <v>54</v>
       </c>
       <c r="E27" s="30">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F27" s="31">
         <v>44000</v>
@@ -6484,7 +6484,7 @@
       <c r="BK27" s="37"/>
       <c r="BL27" s="37"/>
     </row>
-    <row r="28" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="14"/>
       <c r="B28" s="49" t="s">
         <v>50</v>
@@ -6565,7 +6565,7 @@
       <c r="BK28" s="37"/>
       <c r="BL28" s="37"/>
     </row>
-    <row r="29" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
       <c r="B29" s="49" t="s">
         <v>51</v>
@@ -6788,7 +6788,7 @@
         <v/>
       </c>
       <c r="BH29" s="37" t="str">
-        <f t="shared" ref="BH29:BQ30" ca="1" si="27">IF(AND($C28="Goal",BH$5&gt;=$F28,BH$5&lt;=$F28+$G28-1),2,IF(AND($C28="Milestone",BH$5&gt;=$F28,BH$5&lt;=$F28+$G28-1),1,""))</f>
+        <f t="shared" ref="BH29:BL30" ca="1" si="27">IF(AND($C28="Goal",BH$5&gt;=$F28,BH$5&lt;=$F28+$G28-1),2,IF(AND($C28="Milestone",BH$5&gt;=$F28,BH$5&lt;=$F28+$G28-1),1,""))</f>
         <v/>
       </c>
       <c r="BI29" s="37" t="str">
@@ -6808,7 +6808,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="14"/>
       <c r="B30" s="49" t="s">
         <v>53</v>
@@ -7051,7 +7051,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="14"/>
       <c r="B31" s="49" t="s">
         <v>52</v>
@@ -7132,7 +7132,7 @@
       <c r="BK31" s="37"/>
       <c r="BL31" s="37"/>
     </row>
-    <row r="32" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14"/>
       <c r="B32" s="49" t="s">
         <v>69</v>
@@ -7213,7 +7213,7 @@
       <c r="BK32" s="37"/>
       <c r="BL32" s="37"/>
     </row>
-    <row r="33" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="14"/>
       <c r="B33" s="49" t="s">
         <v>70</v>
@@ -7439,7 +7439,7 @@
         <v/>
       </c>
       <c r="BH33" s="37" t="str">
-        <f t="shared" ref="BH33:BQ35" ca="1" si="33">IF(AND($C34="Goal",BH$5&gt;=$F34,BH$5&lt;=$F34+$G34-1),2,IF(AND($C34="Milestone",BH$5&gt;=$F34,BH$5&lt;=$F34+$G34-1),1,""))</f>
+        <f t="shared" ref="BH33:BL35" ca="1" si="33">IF(AND($C34="Goal",BH$5&gt;=$F34,BH$5&lt;=$F34+$G34-1),2,IF(AND($C34="Milestone",BH$5&gt;=$F34,BH$5&lt;=$F34+$G34-1),1,""))</f>
         <v/>
       </c>
       <c r="BI33" s="37" t="str">
@@ -7459,7 +7459,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="14"/>
       <c r="B34" s="57" t="s">
         <v>71</v>
@@ -7702,7 +7702,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="14"/>
       <c r="B35" s="55" t="s">
         <v>38</v>
@@ -7935,7 +7935,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14"/>
       <c r="B36" s="49" t="s">
         <v>38</v>
@@ -8016,7 +8016,7 @@
       <c r="BK36" s="37"/>
       <c r="BL36" s="37"/>
     </row>
-    <row r="37" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="14"/>
       <c r="B37" s="49" t="s">
         <v>48</v>
@@ -8094,7 +8094,7 @@
       <c r="BK37" s="37"/>
       <c r="BL37" s="37"/>
     </row>
-    <row r="38" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="14"/>
       <c r="B38" s="49" t="s">
         <v>49</v>
@@ -8245,7 +8245,7 @@
         <v/>
       </c>
       <c r="AP38" s="37" t="str">
-        <f t="shared" ref="AP38:BU38" ca="1" si="35">IF(AND($C37="Goal",AP$5&gt;=$F37,AP$5&lt;=$F37+$G37-1),2,IF(AND($C37="Milestone",AP$5&gt;=$F37,AP$5&lt;=$F37+$G37-1),1,""))</f>
+        <f t="shared" ref="AP38:BL38" ca="1" si="35">IF(AND($C37="Goal",AP$5&gt;=$F37,AP$5&lt;=$F37+$G37-1),2,IF(AND($C37="Milestone",AP$5&gt;=$F37,AP$5&lt;=$F37+$G37-1),1,""))</f>
         <v/>
       </c>
       <c r="AQ38" s="37" t="str">
@@ -8337,7 +8337,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:64" s="2" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:64" s="2" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="14"/>
       <c r="B39" s="49" t="s">
         <v>45</v>
@@ -8415,7 +8415,7 @@
       <c r="BK39" s="37"/>
       <c r="BL39" s="37"/>
     </row>
-    <row r="40" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="14"/>
       <c r="B40" s="55" t="s">
         <v>36</v>
@@ -8486,7 +8486,7 @@
       <c r="BK40" s="37"/>
       <c r="BL40" s="37"/>
     </row>
-    <row r="41" spans="1:64" s="2" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:64" s="2" customFormat="1" ht="29.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="14"/>
       <c r="B41" s="49" t="s">
         <v>41</v>
@@ -8567,7 +8567,7 @@
       <c r="BK41" s="37"/>
       <c r="BL41" s="37"/>
     </row>
-    <row r="42" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="14"/>
       <c r="B42" s="49" t="s">
         <v>39</v>
@@ -8813,7 +8813,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="14"/>
       <c r="B43" s="49" t="s">
         <v>41</v>
@@ -9059,7 +9059,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="14" t="s">
         <v>2</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:64" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:64" s="2" customFormat="1" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="15" t="s">
         <v>30</v>
       </c>
@@ -9555,7 +9555,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" s="49"/>
       <c r="C46" s="33"/>
       <c r="D46" s="33"/>
@@ -9788,7 +9788,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B47" s="49"/>
       <c r="C47" s="33"/>
       <c r="D47" s="33"/>
@@ -10020,7 +10020,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B48" s="56" t="s">
         <v>18</v>
       </c>
@@ -10254,7 +10254,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="4:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D49" s="5"/>
       <c r="G49" s="16"/>
       <c r="I49" s="37" t="str">
@@ -10482,7 +10482,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="4:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:64" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D50" s="6"/>
       <c r="I50" s="36"/>
       <c r="J50" s="37" t="str">
@@ -10706,7 +10706,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="4:64" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="4:64" ht="30.05" customHeight="1" x14ac:dyDescent="0.35">
       <c r="J51" s="37" t="str">
         <f t="shared" ref="J51:AO51" ca="1" si="55">IF(AND($C47="Goal",J$5&gt;=$F47,J$5&lt;=$F47+$G47-1),2,IF(AND($C47="Milestone",J$5&gt;=$F47,J$5&lt;=$F47+$G47-1),1,""))</f>
         <v/>
@@ -10928,7 +10928,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="4:64" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:64" ht="30.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="J52" s="36"/>
       <c r="K52" s="36"/>
       <c r="L52" s="36"/>
@@ -11213,53 +11213,53 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X22">
-    <cfRule type="expression" dxfId="14" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="11" stopIfTrue="1">
       <formula>AND($C22="Low Risk",X$5&gt;=$F22,X$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="12" stopIfTrue="1">
       <formula>AND($C22="High Risk",X$5&gt;=$F22,X$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="13" stopIfTrue="1">
       <formula>AND($C22="On Track",X$5&gt;=$F22,X$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="14" stopIfTrue="1">
       <formula>AND($C22="Med Risk",X$5&gt;=$F22,X$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
       <formula>AND(LEN($C22)=0,X$5&gt;=$F22,X$5&lt;=$F22+$G22-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X23">
-    <cfRule type="expression" dxfId="9" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
       <formula>AND($C23="Low Risk",X$5&gt;=$F23,X$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>AND($C23="High Risk",X$5&gt;=$F23,X$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>AND($C23="On Track",X$5&gt;=$F23,X$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>AND($C23="Med Risk",X$5&gt;=$F23,X$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="10" stopIfTrue="1">
       <formula>AND(LEN($C23)=0,X$5&gt;=$F23,X$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y23">
-    <cfRule type="expression" dxfId="4" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="1" stopIfTrue="1">
       <formula>AND($C23="Low Risk",Y$5&gt;=$F23,Y$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>AND($C23="High Risk",Y$5&gt;=$F23,Y$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>AND($C23="On Track",Y$5&gt;=$F23,Y$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>AND($C23="Med Risk",Y$5&gt;=$F23,Y$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>AND(LEN($C23)=0,Y$5&gt;=$F23,Y$5&lt;=$F23+$G23-1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11292,15 +11292,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
-                    <xdr:colOff>25400</xdr:colOff>
+                    <xdr:colOff>26314</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>63500</xdr:rowOff>
+                    <xdr:rowOff>65784</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>63</xdr:col>
-                    <xdr:colOff>228600</xdr:colOff>
+                    <xdr:colOff>230245</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>241300</xdr:rowOff>
+                    <xdr:rowOff>243401</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -11451,33 +11451,33 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.95" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="87.1640625" style="10" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="8"/>
+    <col min="1" max="1" width="87.1796875" style="10" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="9" customFormat="1" ht="26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="9" customFormat="1" ht="25.9" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="84.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="84.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="26.3" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" s="10" customFormat="1" ht="205" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>26</v>
       </c>

</xml_diff>